<commit_message>
nuevos cambios y refactorisacion
</commit_message>
<xml_diff>
--- a/app/assets/docs/ENCO_b_Indicador_de_confianza_del_consumidor.xlsx
+++ b/app/assets/docs/ENCO_b_Indicador_de_confianza_del_consumidor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tabulados y Gráficas (Serie histórica)\ENCO0525 Cuadros y Gráficas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB25C6-E077-49B3-8415-ACCE5C87DAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6768340-FA41-4D9A-A213-DCB2F6F87F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1620" windowWidth="28065" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Graficas!$A$2:$O$223</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Total!$A$6:$R$332</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Total!$A$6:$R$333</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Graficas!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Total!$A:$A,Total!$6:$11</definedName>
   </definedNames>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="60">
   <si>
     <t>Periodo</t>
   </si>
@@ -334,7 +334,7 @@
              Encuesta Nacional sobre Confianza del Consumidor (ENCO). Serie mensual enero a marzo 2020 y a partir de agosto 2020</t>
   </si>
   <si>
-    <t>Serie mensual de abril de 2001 a abril de 2025</t>
+    <t>Serie mensual de abril de 2001 a mayo de 2025</t>
   </si>
 </sst>
 </file>
@@ -2202,7 +2202,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:dLblPos val="t"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.9508211682162815E-3"/>
+                  <c:y val="1.5922282441967483E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2753,6 +2759,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>45.454235606749975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.497801253238435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4043,6 +4052,9 @@
                 <c:pt idx="3">
                   <c:v>51.322182008264605</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.174658656033344</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4441,8 +4453,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.3941986331206507E-3"/>
-                  <c:y val="-4.8569383372533614E-3"/>
+                  <c:x val="-4.1445802538281042E-2"/>
+                  <c:y val="1.9385485905170946E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -5198,6 +5210,28 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0181384230736848E-2"/>
+                  <c:y val="-1.5558509731738078E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A7CB-4826-AF01-7D4C791A2730}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -5313,6 +5347,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>56.918498195486343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.493635128706217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6418,6 +6455,28 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.3459844716063215E-4"/>
+                  <c:y val="1.5922282441967483E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-D92C-486A-AF5C-AC19A54A0590}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -6533,6 +6592,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>41.67713215246998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42.044362534747549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7264,7 +7326,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:dLblPos val="b"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.8182204211921211E-2"/>
+                  <c:y val="-2.9099362579677539E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -7877,8 +7945,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.0636986276297053E-2"/>
-                  <c:y val="-3.2874527047755397E-2"/>
+                  <c:x val="-1.947938516053694E-2"/>
+                  <c:y val="3.6389542216313867E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -8132,6 +8200,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>47.111861911639807</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.354541169035905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8992,6 +9063,22 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-EBBA-4084-B099-5D7299752BA3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="6"/>
               <c:dLblPos val="b"/>
               <c:showLegendKey val="0"/>
@@ -9228,6 +9315,22 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-EBBA-4084-B099-5D7299752BA3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -9343,6 +9446,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>30.241503765889185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.421808777669156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12828,13 +12934,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>332</xdr:row>
+      <xdr:row>333</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>332</xdr:row>
+      <xdr:row>333</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -12890,13 +12996,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>331</xdr:row>
+      <xdr:row>332</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>331</xdr:row>
+      <xdr:row>332</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -13517,10 +13623,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:R495"/>
+  <dimension ref="A1:R498"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="11" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:P1"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -27614,66 +27720,94 @@
         <v>-2.6113919397463121</v>
       </c>
     </row>
-    <row r="326" spans="1:18" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A326" s="11"/>
-      <c r="B326" s="81"/>
-      <c r="C326" s="84"/>
-      <c r="D326" s="84"/>
-      <c r="E326" s="59"/>
-      <c r="F326" s="50"/>
-      <c r="G326" s="84"/>
-      <c r="H326" s="59"/>
-      <c r="I326" s="85"/>
-      <c r="J326" s="84"/>
-      <c r="K326" s="59"/>
-      <c r="L326" s="57"/>
-      <c r="M326" s="84"/>
-      <c r="N326" s="59"/>
-      <c r="O326" s="59"/>
-      <c r="P326" s="84"/>
-      <c r="Q326" s="59"/>
-      <c r="R326" s="59"/>
-    </row>
-    <row r="327" spans="1:18" s="4" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A327" s="16"/>
-      <c r="B327" s="32"/>
-      <c r="C327" s="15"/>
-      <c r="D327" s="15"/>
-      <c r="E327" s="48"/>
-      <c r="G327" s="15"/>
-      <c r="H327" s="48"/>
-      <c r="I327" s="83"/>
-      <c r="J327" s="15"/>
-      <c r="K327" s="48"/>
-      <c r="L327" s="58"/>
-      <c r="M327" s="15"/>
-      <c r="N327" s="48"/>
-      <c r="O327" s="48"/>
-      <c r="P327" s="15"/>
-      <c r="Q327" s="48"/>
-      <c r="R327" s="43"/>
-    </row>
-    <row r="328" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A328" s="38" t="s">
-        <v>27</v>
-      </c>
+    <row r="326" spans="1:18" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A326" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B326" s="32">
+        <v>46.497801253238435</v>
+      </c>
+      <c r="C326" s="33">
+        <v>-0.19789345193559882</v>
+      </c>
+      <c r="D326" s="32"/>
+      <c r="E326" s="48">
+        <v>52.174658656033344</v>
+      </c>
+      <c r="F326" s="33">
+        <v>-0.43468489086229312</v>
+      </c>
+      <c r="G326" s="32"/>
+      <c r="H326" s="48">
+        <v>57.493635128706217</v>
+      </c>
+      <c r="I326" s="33">
+        <v>-0.36188032921783986</v>
+      </c>
+      <c r="J326" s="32"/>
+      <c r="K326" s="48">
+        <v>42.044362534747549</v>
+      </c>
+      <c r="L326" s="33">
+        <v>-0.29349798395527671</v>
+      </c>
+      <c r="M326" s="32"/>
+      <c r="N326" s="48">
+        <v>48.354541169035905</v>
+      </c>
+      <c r="O326" s="33">
+        <v>-1.0597476934033168</v>
+      </c>
+      <c r="P326" s="32"/>
+      <c r="Q326" s="48">
+        <v>32.421808777669156</v>
+      </c>
+      <c r="R326" s="33">
+        <v>1.1603436377607181</v>
+      </c>
+    </row>
+    <row r="327" spans="1:18" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="11"/>
+      <c r="B327" s="81"/>
+      <c r="C327" s="84"/>
+      <c r="D327" s="84"/>
+      <c r="E327" s="59"/>
+      <c r="F327" s="50"/>
+      <c r="G327" s="84"/>
+      <c r="H327" s="59"/>
+      <c r="I327" s="85"/>
+      <c r="J327" s="84"/>
+      <c r="K327" s="59"/>
+      <c r="L327" s="57"/>
+      <c r="M327" s="84"/>
+      <c r="N327" s="59"/>
+      <c r="O327" s="59"/>
+      <c r="P327" s="84"/>
+      <c r="Q327" s="59"/>
+      <c r="R327" s="59"/>
+    </row>
+    <row r="328" spans="1:18" s="4" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="16"/>
       <c r="B328" s="32"/>
-      <c r="C328" s="39"/>
-      <c r="D328" s="39"/>
+      <c r="C328" s="15"/>
+      <c r="D328" s="15"/>
       <c r="E328" s="48"/>
-      <c r="F328" s="39"/>
-      <c r="G328" s="39"/>
+      <c r="G328" s="15"/>
       <c r="H328" s="48"/>
-      <c r="J328" s="39"/>
+      <c r="I328" s="83"/>
+      <c r="J328" s="15"/>
       <c r="K328" s="48"/>
-      <c r="M328" s="39"/>
+      <c r="L328" s="58"/>
+      <c r="M328" s="15"/>
       <c r="N328" s="48"/>
-      <c r="P328" s="39"/>
+      <c r="O328" s="48"/>
+      <c r="P328" s="15"/>
       <c r="Q328" s="48"/>
+      <c r="R328" s="43"/>
     </row>
     <row r="329" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="38" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B329" s="32"/>
       <c r="C329" s="39"/>
@@ -27689,31 +27823,27 @@
       <c r="P329" s="39"/>
       <c r="Q329" s="48"/>
     </row>
-    <row r="330" spans="1:18" s="40" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="89" t="s">
+    <row r="330" spans="1:18" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B330" s="32"/>
+      <c r="C330" s="39"/>
+      <c r="D330" s="39"/>
+      <c r="E330" s="48"/>
+      <c r="F330" s="39"/>
+      <c r="G330" s="39"/>
+      <c r="H330" s="48"/>
+      <c r="J330" s="39"/>
+      <c r="K330" s="48"/>
+      <c r="M330" s="39"/>
+      <c r="N330" s="48"/>
+      <c r="P330" s="39"/>
+      <c r="Q330" s="48"/>
+    </row>
+    <row r="331" spans="1:18" s="40" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="89" t="s">
         <v>56</v>
-      </c>
-      <c r="B330" s="89"/>
-      <c r="C330" s="89"/>
-      <c r="D330" s="89"/>
-      <c r="E330" s="89"/>
-      <c r="F330" s="89"/>
-      <c r="G330" s="89"/>
-      <c r="H330" s="89"/>
-      <c r="I330" s="89"/>
-      <c r="J330" s="89"/>
-      <c r="K330" s="89"/>
-      <c r="L330" s="89"/>
-      <c r="M330" s="89"/>
-      <c r="N330" s="89"/>
-      <c r="O330" s="89"/>
-      <c r="P330" s="89"/>
-      <c r="Q330" s="89"/>
-      <c r="R330" s="89"/>
-    </row>
-    <row r="331" spans="1:18" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A331" s="89" t="s">
-        <v>54</v>
       </c>
       <c r="B331" s="89"/>
       <c r="C331" s="89"/>
@@ -27733,9 +27863,9 @@
       <c r="Q331" s="89"/>
       <c r="R331" s="89"/>
     </row>
-    <row r="332" spans="1:18" s="42" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:18" s="40" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="89" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B332" s="89"/>
       <c r="C332" s="89"/>
@@ -27755,162 +27885,195 @@
       <c r="Q332" s="89"/>
       <c r="R332" s="89"/>
     </row>
-    <row r="333" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B333" s="32"/>
-      <c r="C333" s="32"/>
-      <c r="E333" s="48"/>
-      <c r="F333" s="52"/>
-      <c r="H333" s="48"/>
-      <c r="K333" s="48"/>
-      <c r="L333" s="51"/>
-      <c r="N333" s="48"/>
-      <c r="O333" s="51"/>
-      <c r="Q333" s="48"/>
-    </row>
-    <row r="334" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:18" s="42" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A333" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="B333" s="89"/>
+      <c r="C333" s="89"/>
+      <c r="D333" s="89"/>
+      <c r="E333" s="89"/>
+      <c r="F333" s="89"/>
+      <c r="G333" s="89"/>
+      <c r="H333" s="89"/>
+      <c r="I333" s="89"/>
+      <c r="J333" s="89"/>
+      <c r="K333" s="89"/>
+      <c r="L333" s="89"/>
+      <c r="M333" s="89"/>
+      <c r="N333" s="89"/>
+      <c r="O333" s="89"/>
+      <c r="P333" s="89"/>
+      <c r="Q333" s="89"/>
+      <c r="R333" s="89"/>
+    </row>
+    <row r="334" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B334" s="32"/>
+      <c r="C334" s="32"/>
       <c r="E334" s="48"/>
+      <c r="F334" s="52"/>
       <c r="H334" s="48"/>
       <c r="K334" s="48"/>
       <c r="L334" s="51"/>
       <c r="N334" s="48"/>
-      <c r="O334" s="53"/>
+      <c r="O334" s="51"/>
       <c r="Q334" s="48"/>
-      <c r="R334"/>
-    </row>
-    <row r="335" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B335" s="18"/>
-      <c r="E335" s="82"/>
-      <c r="H335" s="4"/>
-      <c r="K335" s="58"/>
+    </row>
+    <row r="335" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="B335" s="32"/>
+      <c r="E335" s="48"/>
+      <c r="H335" s="48"/>
+      <c r="K335" s="48"/>
       <c r="L335" s="51"/>
       <c r="N335" s="48"/>
+      <c r="O335" s="53"/>
       <c r="Q335" s="48"/>
+      <c r="R335"/>
     </row>
     <row r="336" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B336" s="15"/>
-      <c r="E336" s="4"/>
-      <c r="H336" s="38"/>
-      <c r="K336" s="58"/>
+      <c r="B336" s="32"/>
+      <c r="E336" s="48"/>
+      <c r="H336" s="48"/>
+      <c r="K336" s="48"/>
       <c r="L336" s="51"/>
       <c r="N336" s="48"/>
-      <c r="Q336" s="42"/>
+      <c r="O336"/>
+      <c r="Q336" s="48"/>
     </row>
     <row r="337" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B337" s="39"/>
-      <c r="E337" s="39"/>
-      <c r="H337" s="40"/>
-      <c r="K337" s="40"/>
+      <c r="B337" s="32"/>
+      <c r="E337" s="48"/>
+      <c r="H337" s="48"/>
+      <c r="K337" s="48"/>
       <c r="L337" s="51"/>
-      <c r="N337" s="40"/>
-      <c r="Q337" s="40"/>
+      <c r="N337" s="48"/>
+      <c r="O337" s="42"/>
+      <c r="Q337" s="48"/>
     </row>
     <row r="338" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B338" s="38"/>
-      <c r="E338" s="80"/>
-      <c r="H338" s="80"/>
-      <c r="K338" s="42"/>
+      <c r="B338" s="18"/>
+      <c r="E338" s="82"/>
+      <c r="H338" s="4"/>
+      <c r="K338" s="58"/>
       <c r="L338" s="51"/>
-      <c r="N338" s="42"/>
-      <c r="Q338" s="42"/>
+      <c r="N338" s="48"/>
+      <c r="Q338" s="48"/>
     </row>
     <row r="339" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B339" s="15"/>
+      <c r="E339" s="4"/>
+      <c r="H339" s="38"/>
+      <c r="K339" s="58"/>
       <c r="L339" s="51"/>
-      <c r="N339" s="38"/>
+      <c r="N339" s="48"/>
+      <c r="Q339" s="42"/>
     </row>
     <row r="340" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B340" s="39"/>
+      <c r="E340" s="39"/>
+      <c r="H340" s="40"/>
+      <c r="K340" s="40"/>
       <c r="L340" s="51"/>
+      <c r="N340" s="40"/>
+      <c r="Q340" s="40"/>
     </row>
     <row r="341" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B341" s="38"/>
+      <c r="E341" s="80"/>
+      <c r="H341" s="80"/>
+      <c r="K341" s="42"/>
       <c r="L341" s="51"/>
+      <c r="N341" s="42"/>
+      <c r="Q341" s="42"/>
     </row>
     <row r="342" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L342" s="51"/>
-      <c r="Q342"/>
+      <c r="N342" s="38"/>
     </row>
     <row r="343" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L343" s="51"/>
-      <c r="Q343"/>
     </row>
     <row r="344" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L344" s="51"/>
-      <c r="Q344"/>
     </row>
     <row r="345" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L345" s="51"/>
-      <c r="Q345" s="42"/>
+      <c r="Q345"/>
     </row>
     <row r="346" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L346" s="51"/>
+      <c r="Q346"/>
     </row>
     <row r="347" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L347" s="51"/>
+      <c r="Q347"/>
     </row>
     <row r="348" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L348" s="51"/>
-      <c r="N348"/>
+      <c r="Q348" s="42"/>
     </row>
     <row r="349" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L349" s="51"/>
-      <c r="N349"/>
     </row>
     <row r="350" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L350" s="51"/>
-      <c r="N350"/>
     </row>
     <row r="351" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L351" s="51"/>
-      <c r="N351" s="42"/>
+      <c r="N351"/>
     </row>
     <row r="352" spans="2:17" x14ac:dyDescent="0.2">
       <c r="L352" s="51"/>
-    </row>
-    <row r="353" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="N352"/>
+    </row>
+    <row r="353" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L353" s="51"/>
-    </row>
-    <row r="354" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="N353"/>
+    </row>
+    <row r="354" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L354" s="51"/>
-    </row>
-    <row r="355" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="N354" s="42"/>
+    </row>
+    <row r="355" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L355" s="51"/>
     </row>
-    <row r="356" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="356" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L356" s="51"/>
     </row>
-    <row r="357" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="357" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L357" s="51"/>
     </row>
-    <row r="358" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="358" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L358" s="51"/>
     </row>
-    <row r="359" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="359" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L359" s="51"/>
     </row>
-    <row r="360" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="360" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L360" s="51"/>
     </row>
-    <row r="361" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="361" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L361" s="51"/>
     </row>
-    <row r="362" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="362" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L362" s="51"/>
     </row>
-    <row r="363" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="363" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L363" s="51"/>
     </row>
-    <row r="364" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="364" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L364" s="51"/>
     </row>
-    <row r="365" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="365" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L365" s="51"/>
     </row>
-    <row r="366" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="366" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L366" s="51"/>
     </row>
-    <row r="367" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="367" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L367" s="51"/>
     </row>
-    <row r="368" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="368" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L368" s="51"/>
     </row>
     <row r="369" spans="12:12" x14ac:dyDescent="0.2">
@@ -28294,9 +28457,18 @@
     <row r="495" spans="12:12" x14ac:dyDescent="0.2">
       <c r="L495" s="51"/>
     </row>
+    <row r="496" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L496" s="51"/>
+    </row>
+    <row r="497" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L497" s="51"/>
+    </row>
+    <row r="498" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L498" s="51"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A332:R332"/>
+    <mergeCell ref="A333:R333"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="E9:F9"/>
@@ -28305,8 +28477,8 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="A332:R332"/>
     <mergeCell ref="A331:R331"/>
-    <mergeCell ref="A330:R330"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.59055118110236227" bottom="0.70866141732283472" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -28586,7 +28758,9 @@
       <c r="F12" s="87">
         <v>45.454235606749975</v>
       </c>
-      <c r="G12" s="87"/>
+      <c r="G12" s="87">
+        <v>46.497801253238435</v>
+      </c>
       <c r="H12" s="87"/>
       <c r="I12" s="87"/>
       <c r="J12" s="87"/>
@@ -28904,7 +29078,9 @@
       <c r="F49" s="87">
         <v>51.322182008264605</v>
       </c>
-      <c r="G49" s="87"/>
+      <c r="G49" s="87">
+        <v>52.174658656033344</v>
+      </c>
       <c r="H49" s="87"/>
       <c r="I49" s="87"/>
       <c r="J49" s="87"/>
@@ -29239,7 +29415,9 @@
       <c r="F86" s="87">
         <v>56.918498195486343</v>
       </c>
-      <c r="G86" s="87"/>
+      <c r="G86" s="87">
+        <v>57.493635128706217</v>
+      </c>
       <c r="H86" s="87"/>
       <c r="I86" s="87"/>
       <c r="J86" s="87"/>
@@ -29574,7 +29752,9 @@
       <c r="F123" s="87">
         <v>41.67713215246998</v>
       </c>
-      <c r="G123" s="87"/>
+      <c r="G123" s="87">
+        <v>42.044362534747549</v>
+      </c>
       <c r="H123" s="87"/>
       <c r="I123" s="87"/>
       <c r="J123" s="87"/>
@@ -29909,7 +30089,9 @@
       <c r="F160" s="87">
         <v>47.111861911639807</v>
       </c>
-      <c r="G160" s="87"/>
+      <c r="G160" s="87">
+        <v>48.354541169035905</v>
+      </c>
       <c r="H160" s="87"/>
       <c r="I160" s="87"/>
       <c r="J160" s="87"/>
@@ -30244,7 +30426,9 @@
       <c r="F197" s="87">
         <v>30.241503765889185</v>
       </c>
-      <c r="G197" s="87"/>
+      <c r="G197" s="87">
+        <v>32.421808777669156</v>
+      </c>
       <c r="H197" s="87"/>
       <c r="I197" s="87"/>
       <c r="J197" s="87"/>

</xml_diff>